<commit_message>
update on team's names
</commit_message>
<xml_diff>
--- a/file/old.xlsx
+++ b/file/old.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckkil\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckkil\Documents\GitHub\cs-tools\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB498142-1BAB-4AE9-92FD-5FE2716850D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA7BC3B-0CC8-4FCA-8168-B9F0D0C551C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="2160" windowWidth="15525" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15525" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DHW 25 - Stage 1" sheetId="1" r:id="rId1"/>
@@ -427,9 +427,6 @@
     <t>Quantum Bellator Fire</t>
   </si>
   <si>
-    <t>Reason Gaming</t>
-  </si>
-  <si>
     <t>Rebels</t>
   </si>
   <si>
@@ -484,12 +481,6 @@
     <t>TALON</t>
   </si>
   <si>
-    <t>Team Kinguin</t>
-  </si>
-  <si>
-    <t>Team Solid</t>
-  </si>
-  <si>
     <t>The Dice</t>
   </si>
   <si>
@@ -557,6 +548,15 @@
   </si>
   <si>
     <t>Wizards</t>
+  </si>
+  <si>
+    <t>Solid</t>
+  </si>
+  <si>
+    <t>Kinguin</t>
+  </si>
+  <si>
+    <t>Reason</t>
   </si>
 </sst>
 </file>
@@ -598,11 +598,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -942,8 +944,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4833,7 +4835,7 @@
     </row>
     <row r="122" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>134</v>
+        <v>177</v>
       </c>
       <c r="B122" s="7">
         <v>0</v>
@@ -4865,7 +4867,7 @@
     </row>
     <row r="123" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B123" s="7">
         <v>0</v>
@@ -4897,7 +4899,7 @@
     </row>
     <row r="124" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A124" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B124" s="7">
         <v>6</v>
@@ -4929,7 +4931,7 @@
     </row>
     <row r="125" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A125" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B125" s="7">
         <v>0</v>
@@ -4961,7 +4963,7 @@
     </row>
     <row r="126" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A126" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B126" s="7">
         <v>0</v>
@@ -4993,7 +4995,7 @@
     </row>
     <row r="127" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A127" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B127" s="7">
         <v>0</v>
@@ -5025,7 +5027,7 @@
     </row>
     <row r="128" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B128" s="7">
         <v>0</v>
@@ -5057,7 +5059,7 @@
     </row>
     <row r="129" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A129" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B129" s="7">
         <v>0</v>
@@ -5089,7 +5091,7 @@
     </row>
     <row r="130" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A130" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B130" s="7">
         <v>0</v>
@@ -5121,7 +5123,7 @@
     </row>
     <row r="131" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B131" s="7">
         <v>0</v>
@@ -5153,7 +5155,7 @@
     </row>
     <row r="132" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A132" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B132" s="7">
         <v>3</v>
@@ -5185,7 +5187,7 @@
     </row>
     <row r="133" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A133" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B133" s="7">
         <v>0</v>
@@ -5217,7 +5219,7 @@
     </row>
     <row r="134" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B134" s="7">
         <v>0</v>
@@ -5249,7 +5251,7 @@
     </row>
     <row r="135" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A135" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B135" s="7">
         <v>0</v>
@@ -5281,7 +5283,7 @@
     </row>
     <row r="136" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A136" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B136" s="7">
         <v>0</v>
@@ -5313,7 +5315,7 @@
     </row>
     <row r="137" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B137" s="7">
         <v>0</v>
@@ -5345,7 +5347,7 @@
     </row>
     <row r="138" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A138" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B138" s="7">
         <v>0</v>
@@ -5377,7 +5379,7 @@
     </row>
     <row r="139" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A139" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B139" s="7">
         <v>0</v>
@@ -5409,7 +5411,7 @@
     </row>
     <row r="140" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A140" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B140" s="7">
         <v>0</v>
@@ -5441,7 +5443,7 @@
     </row>
     <row r="141" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A141" s="11" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="B141" s="7">
         <v>0</v>
@@ -5473,7 +5475,7 @@
     </row>
     <row r="142" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A142" s="12" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="B142" s="7">
         <v>0</v>
@@ -5505,7 +5507,7 @@
     </row>
     <row r="143" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A143" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B143" s="7">
         <v>0</v>
@@ -5537,7 +5539,7 @@
     </row>
     <row r="144" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A144" s="12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B144" s="7">
         <v>0</v>
@@ -5569,7 +5571,7 @@
     </row>
     <row r="145" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A145" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B145" s="7">
         <v>0</v>
@@ -5601,7 +5603,7 @@
     </row>
     <row r="146" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A146" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B146" s="7">
         <v>10</v>
@@ -5633,7 +5635,7 @@
     </row>
     <row r="147" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A147" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B147" s="7">
         <v>0</v>
@@ -5665,7 +5667,7 @@
     </row>
     <row r="148" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A148" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B148" s="7">
         <v>0</v>
@@ -5697,7 +5699,7 @@
     </row>
     <row r="149" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A149" s="13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B149" s="7">
         <v>0</v>
@@ -5729,7 +5731,7 @@
     </row>
     <row r="150" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A150" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B150" s="7">
         <v>0</v>
@@ -5761,7 +5763,7 @@
     </row>
     <row r="151" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A151" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B151" s="7">
         <v>0</v>
@@ -5793,7 +5795,7 @@
     </row>
     <row r="152" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A152" s="13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B152" s="7">
         <v>0</v>
@@ -5825,7 +5827,7 @@
     </row>
     <row r="153" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A153" s="12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B153" s="7">
         <v>0</v>
@@ -5857,7 +5859,7 @@
     </row>
     <row r="154" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A154" s="13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B154" s="7">
         <v>11</v>
@@ -5889,7 +5891,7 @@
     </row>
     <row r="155" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A155" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B155" s="7">
         <v>0</v>
@@ -5921,7 +5923,7 @@
     </row>
     <row r="156" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A156" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B156" s="7">
         <v>0</v>
@@ -5953,7 +5955,7 @@
     </row>
     <row r="157" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A157" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B157" s="7">
         <v>0</v>
@@ -5985,7 +5987,7 @@
     </row>
     <row r="158" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A158" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B158" s="7">
         <v>0</v>
@@ -6017,7 +6019,7 @@
     </row>
     <row r="159" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A159" s="11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B159" s="7">
         <v>0</v>
@@ -6049,7 +6051,7 @@
     </row>
     <row r="160" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A160" s="13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B160" s="7">
         <v>0</v>
@@ -6081,7 +6083,7 @@
     </row>
     <row r="161" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A161" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B161" s="7">
         <v>0</v>
@@ -6113,7 +6115,7 @@
     </row>
     <row r="162" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A162" s="12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B162" s="7">
         <v>0</v>
@@ -6145,7 +6147,7 @@
     </row>
     <row r="163" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A163" s="11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B163" s="7">
         <v>0</v>
@@ -6177,7 +6179,7 @@
     </row>
     <row r="164" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A164" s="13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B164" s="7">
         <v>0</v>
@@ -6209,7 +6211,7 @@
     </row>
     <row r="165" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A165" s="12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B165" s="7">
         <v>3</v>

</xml_diff>